<commit_message>
Balanced some stuff, placed order.
</commit_message>
<xml_diff>
--- a/Gimmix/MS Exp Curve.xlsx
+++ b/Gimmix/MS Exp Curve.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Creature</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Ensnaring Bridge?</t>
+  </si>
+  <si>
+    <t>Skill Dmg</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1640,11 +1642,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="277733464"/>
-        <c:axId val="277733072"/>
+        <c:axId val="289646936"/>
+        <c:axId val="289647328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="277733464"/>
+        <c:axId val="289646936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1687,7 +1689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277733072"/>
+        <c:crossAx val="289647328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1695,7 +1697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277733072"/>
+        <c:axId val="289647328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277733464"/>
+        <c:crossAx val="289646936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2859,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2879,6 +2881,9 @@
       <c r="M1" t="s">
         <v>17</v>
       </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" t="s">
@@ -2934,7 +2939,7 @@
         <v>25</v>
       </c>
       <c r="Y3">
-        <f>ROUNDUP(SUM((-0.0949*B3)+18.0949),0)</f>
+        <f>ROUNDUP(SUM((-0.09*B3)+18),0)</f>
         <v>18</v>
       </c>
     </row>
@@ -2943,11 +2948,11 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C67" si="0">ROUNDDOWN(SUM((B4*5)+8 +Y4),0)</f>
+        <f t="shared" ref="C4:C51" si="0">ROUNDDOWN(SUM((B4*5)+8 +Y4),0)</f>
         <v>36</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D67" si="1">ROUNDDOWN(SUM((B4/2)+4),0)</f>
+        <f t="shared" ref="D4:D51" si="1">ROUNDDOWN(SUM((B4/2)+4),0)</f>
         <v>5</v>
       </c>
       <c r="E4">
@@ -2969,7 +2974,7 @@
         <v>31</v>
       </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y67" si="3">ROUNDUP(SUM((-0.0949*B4)+18.0949),0)</f>
+        <f t="shared" ref="Y4:Y67" si="3">ROUNDUP(SUM((-0.09*B4)+18),0)</f>
         <v>18</v>
       </c>
     </row>
@@ -4029,7 +4034,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
@@ -4047,15 +4052,15 @@
       </c>
       <c r="K35">
         <f>ROUNDDOWN(SUM(0.5*M35),0)</f>
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M35">
         <f t="shared" si="5"/>
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="Y35">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="2:25">
@@ -4414,7 +4419,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
@@ -4432,15 +4437,15 @@
       </c>
       <c r="K46">
         <f t="shared" si="7"/>
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="M46">
         <f t="shared" si="5"/>
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="Y46">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="2:25">
@@ -4764,7 +4769,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="8"/>
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D56">
         <f t="shared" si="9"/>
@@ -4782,15 +4787,15 @@
       </c>
       <c r="K56">
         <f t="shared" si="7"/>
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="M56">
         <f t="shared" si="5"/>
-        <v>1410</v>
+        <v>1415</v>
       </c>
       <c r="Y56">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="2:25">
@@ -4799,7 +4804,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="8"/>
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D57">
         <f t="shared" si="9"/>
@@ -4817,15 +4822,15 @@
       </c>
       <c r="K57">
         <f t="shared" si="7"/>
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="M57">
         <f t="shared" si="5"/>
-        <v>1461</v>
+        <v>1466</v>
       </c>
       <c r="Y57">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="2:25">
@@ -5149,7 +5154,7 @@
       </c>
       <c r="C67">
         <f t="shared" si="8"/>
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D67">
         <f t="shared" si="9"/>
@@ -5167,15 +5172,15 @@
       </c>
       <c r="K67">
         <f t="shared" si="7"/>
-        <v>1210</v>
+        <v>1213</v>
       </c>
       <c r="M67">
         <f t="shared" si="5"/>
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="Y67">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="2:25">
@@ -5184,7 +5189,7 @@
       </c>
       <c r="C68">
         <f t="shared" si="8"/>
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D68">
         <f t="shared" si="9"/>
@@ -5202,15 +5207,15 @@
       </c>
       <c r="K68">
         <f t="shared" si="7"/>
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="M68">
         <f t="shared" si="5"/>
-        <v>2095</v>
+        <v>2101</v>
       </c>
       <c r="Y68">
-        <f t="shared" ref="Y68:Y131" si="10">ROUNDUP(SUM((-0.0949*B68)+18.0949),0)</f>
-        <v>12</v>
+        <f t="shared" ref="Y68:Y131" si="10">ROUNDUP(SUM((-0.09*B68)+18),0)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="2:25">
@@ -5499,7 +5504,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="8"/>
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D77">
         <f t="shared" si="9"/>
@@ -5517,15 +5522,15 @@
       </c>
       <c r="K77">
         <f t="shared" si="7"/>
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="M77">
         <f t="shared" si="11"/>
-        <v>2717</v>
+        <v>2723</v>
       </c>
       <c r="Y77">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="2:25">
@@ -5534,7 +5539,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="8"/>
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D78">
         <f t="shared" si="9"/>
@@ -5552,15 +5557,15 @@
       </c>
       <c r="K78">
         <f t="shared" si="7"/>
-        <v>1672</v>
+        <v>1677</v>
       </c>
       <c r="M78">
         <f t="shared" si="11"/>
-        <v>2788</v>
+        <v>2795</v>
       </c>
       <c r="Y78">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="2:25">
@@ -5569,7 +5574,7 @@
       </c>
       <c r="C79">
         <f t="shared" si="8"/>
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D79">
         <f t="shared" si="9"/>
@@ -5587,15 +5592,15 @@
       </c>
       <c r="K79">
         <f t="shared" si="7"/>
-        <v>1726</v>
+        <v>1731</v>
       </c>
       <c r="M79">
         <f t="shared" si="11"/>
-        <v>2878</v>
+        <v>2885</v>
       </c>
       <c r="Y79">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="2:25">
@@ -5884,7 +5889,7 @@
       </c>
       <c r="C88">
         <f t="shared" si="8"/>
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D88">
         <f t="shared" si="9"/>
@@ -5902,15 +5907,15 @@
       </c>
       <c r="K88">
         <f t="shared" si="7"/>
-        <v>2185</v>
+        <v>2189</v>
       </c>
       <c r="M88">
         <f t="shared" si="11"/>
-        <v>3642</v>
+        <v>3649</v>
       </c>
       <c r="Y88">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="2:25">
@@ -5919,7 +5924,7 @@
       </c>
       <c r="C89">
         <f t="shared" si="8"/>
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D89">
         <f t="shared" si="9"/>
@@ -5937,15 +5942,15 @@
       </c>
       <c r="K89">
         <f t="shared" si="7"/>
-        <v>2233</v>
+        <v>2238</v>
       </c>
       <c r="M89">
         <f t="shared" si="11"/>
-        <v>3722</v>
+        <v>3730</v>
       </c>
       <c r="Y89">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="2:25">
@@ -5954,7 +5959,7 @@
       </c>
       <c r="C90">
         <f t="shared" si="8"/>
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D90">
         <f t="shared" si="9"/>
@@ -5972,15 +5977,15 @@
       </c>
       <c r="K90">
         <f t="shared" si="7"/>
-        <v>2296</v>
+        <v>2301</v>
       </c>
       <c r="M90">
         <f t="shared" si="11"/>
-        <v>3827</v>
+        <v>3835</v>
       </c>
       <c r="Y90">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="2:25">
@@ -6234,7 +6239,7 @@
       </c>
       <c r="C98">
         <f t="shared" si="8"/>
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D98">
         <f t="shared" si="9"/>
@@ -6252,15 +6257,15 @@
       </c>
       <c r="K98">
         <f t="shared" si="7"/>
-        <v>2763</v>
+        <v>2769</v>
       </c>
       <c r="M98">
         <f t="shared" si="11"/>
-        <v>4606</v>
+        <v>4615</v>
       </c>
       <c r="Y98">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="2:25">
@@ -6269,7 +6274,7 @@
       </c>
       <c r="C99">
         <f t="shared" si="8"/>
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D99">
         <f t="shared" si="9"/>
@@ -6287,15 +6292,15 @@
       </c>
       <c r="K99">
         <f t="shared" si="7"/>
-        <v>2832</v>
+        <v>2837</v>
       </c>
       <c r="M99">
         <f t="shared" si="11"/>
-        <v>4720</v>
+        <v>4729</v>
       </c>
       <c r="Y99">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="2:25">
@@ -6304,7 +6309,7 @@
       </c>
       <c r="C100">
         <f t="shared" si="8"/>
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D100">
         <f t="shared" si="9"/>
@@ -6322,15 +6327,15 @@
       </c>
       <c r="K100">
         <f t="shared" si="7"/>
-        <v>2902</v>
+        <v>2908</v>
       </c>
       <c r="M100">
         <f t="shared" si="11"/>
-        <v>4838</v>
+        <v>4847</v>
       </c>
       <c r="Y100">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="2:25">
@@ -6339,7 +6344,7 @@
       </c>
       <c r="C101">
         <f t="shared" si="8"/>
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D101">
         <f t="shared" si="9"/>
@@ -6357,15 +6362,15 @@
       </c>
       <c r="K101">
         <f t="shared" si="7"/>
-        <v>2958</v>
+        <v>2963</v>
       </c>
       <c r="M101">
         <f t="shared" si="11"/>
-        <v>4930</v>
+        <v>4939</v>
       </c>
       <c r="Y101">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="2:25">
@@ -6619,7 +6624,7 @@
       </c>
       <c r="C109">
         <f t="shared" si="8"/>
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D109">
         <f t="shared" si="9"/>
@@ -6637,15 +6642,15 @@
       </c>
       <c r="K109">
         <f t="shared" si="13"/>
-        <v>3530</v>
+        <v>3536</v>
       </c>
       <c r="M109">
         <f t="shared" si="11"/>
-        <v>5884</v>
+        <v>5894</v>
       </c>
       <c r="Y109">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="2:25">
@@ -6654,7 +6659,7 @@
       </c>
       <c r="C110">
         <f t="shared" si="8"/>
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D110">
         <f t="shared" si="9"/>
@@ -6672,15 +6677,15 @@
       </c>
       <c r="K110">
         <f t="shared" si="13"/>
-        <v>3609</v>
+        <v>3615</v>
       </c>
       <c r="M110">
         <f t="shared" si="11"/>
-        <v>6015</v>
+        <v>6025</v>
       </c>
       <c r="Y110">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="2:25">
@@ -6689,7 +6694,7 @@
       </c>
       <c r="C111">
         <f t="shared" si="8"/>
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D111">
         <f t="shared" si="9"/>
@@ -6707,15 +6712,15 @@
       </c>
       <c r="K111">
         <f t="shared" si="13"/>
-        <v>3670</v>
+        <v>3676</v>
       </c>
       <c r="M111">
         <f t="shared" si="11"/>
-        <v>6118</v>
+        <v>6128</v>
       </c>
       <c r="Y111">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="2:25">
@@ -6724,7 +6729,7 @@
       </c>
       <c r="C112">
         <f t="shared" si="8"/>
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D112">
         <f t="shared" si="9"/>
@@ -6742,15 +6747,15 @@
       </c>
       <c r="K112">
         <f t="shared" si="13"/>
-        <v>3750</v>
+        <v>3757</v>
       </c>
       <c r="M112">
         <f t="shared" si="11"/>
-        <v>6251</v>
+        <v>6262</v>
       </c>
       <c r="Y112">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="2:25">
@@ -6759,7 +6764,7 @@
       </c>
       <c r="C113">
         <f t="shared" si="8"/>
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D113">
         <f t="shared" si="9"/>
@@ -6777,15 +6782,15 @@
       </c>
       <c r="K113">
         <f t="shared" si="13"/>
-        <v>3829</v>
+        <v>3836</v>
       </c>
       <c r="M113">
         <f t="shared" si="11"/>
-        <v>6383</v>
+        <v>6394</v>
       </c>
       <c r="Y113">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="2:25">
@@ -6969,7 +6974,7 @@
       </c>
       <c r="C119">
         <f t="shared" si="14"/>
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D119">
         <f t="shared" si="15"/>
@@ -6987,15 +6992,15 @@
       </c>
       <c r="K119">
         <f t="shared" si="13"/>
-        <v>4320</v>
+        <v>4326</v>
       </c>
       <c r="M119">
         <f t="shared" si="11"/>
-        <v>7200</v>
+        <v>7211</v>
       </c>
       <c r="Y119">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="2:25">
@@ -7004,7 +7009,7 @@
       </c>
       <c r="C120">
         <f t="shared" si="14"/>
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D120">
         <f t="shared" si="15"/>
@@ -7022,15 +7027,15 @@
       </c>
       <c r="K120">
         <f t="shared" si="13"/>
-        <v>4406</v>
+        <v>4413</v>
       </c>
       <c r="M120">
         <f t="shared" si="11"/>
-        <v>7344</v>
+        <v>7355</v>
       </c>
       <c r="Y120">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="2:25">
@@ -7039,7 +7044,7 @@
       </c>
       <c r="C121">
         <f t="shared" si="14"/>
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D121">
         <f t="shared" si="15"/>
@@ -7057,15 +7062,15 @@
       </c>
       <c r="K121">
         <f t="shared" si="13"/>
-        <v>4491</v>
+        <v>4498</v>
       </c>
       <c r="M121">
         <f t="shared" si="11"/>
-        <v>7486</v>
+        <v>7498</v>
       </c>
       <c r="Y121">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="2:25">
@@ -7074,7 +7079,7 @@
       </c>
       <c r="C122">
         <f t="shared" si="14"/>
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D122">
         <f t="shared" si="15"/>
@@ -7092,15 +7097,15 @@
       </c>
       <c r="K122">
         <f t="shared" si="13"/>
-        <v>4579</v>
+        <v>4587</v>
       </c>
       <c r="M122">
         <f t="shared" si="11"/>
-        <v>7633</v>
+        <v>7645</v>
       </c>
       <c r="Y122">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="2:25">
@@ -7109,7 +7114,7 @@
       </c>
       <c r="C123">
         <f t="shared" si="14"/>
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D123">
         <f t="shared" si="15"/>
@@ -7127,15 +7132,15 @@
       </c>
       <c r="K123">
         <f t="shared" si="13"/>
-        <v>4666</v>
+        <v>4674</v>
       </c>
       <c r="M123">
         <f t="shared" si="11"/>
-        <v>7778</v>
+        <v>7790</v>
       </c>
       <c r="Y123">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="2:25">
@@ -7144,7 +7149,7 @@
       </c>
       <c r="C124">
         <f t="shared" si="14"/>
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D124">
         <f t="shared" si="15"/>
@@ -7162,15 +7167,15 @@
       </c>
       <c r="K124">
         <f t="shared" si="13"/>
-        <v>4756</v>
+        <v>4763</v>
       </c>
       <c r="M124">
         <f t="shared" si="11"/>
-        <v>7927</v>
+        <v>7939</v>
       </c>
       <c r="Y124">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="2:25">
@@ -7354,7 +7359,7 @@
       </c>
       <c r="C130">
         <f t="shared" si="14"/>
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D130">
         <f t="shared" si="15"/>
@@ -7372,15 +7377,15 @@
       </c>
       <c r="K130">
         <f t="shared" si="13"/>
-        <v>5316</v>
+        <v>5324</v>
       </c>
       <c r="M130">
         <f t="shared" si="11"/>
-        <v>8861</v>
+        <v>8874</v>
       </c>
       <c r="Y130">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="2:25">
@@ -7389,7 +7394,7 @@
       </c>
       <c r="C131">
         <f t="shared" si="14"/>
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D131">
         <f t="shared" si="15"/>
@@ -7407,15 +7412,15 @@
       </c>
       <c r="K131">
         <f t="shared" si="13"/>
-        <v>5410</v>
+        <v>5418</v>
       </c>
       <c r="M131">
         <f t="shared" si="11"/>
-        <v>9017</v>
+        <v>9030</v>
       </c>
       <c r="Y131">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="2:25">
@@ -7424,7 +7429,7 @@
       </c>
       <c r="C132">
         <f t="shared" si="14"/>
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D132">
         <f t="shared" si="15"/>
@@ -7442,15 +7447,15 @@
       </c>
       <c r="K132">
         <f t="shared" si="13"/>
-        <v>5506</v>
+        <v>5514</v>
       </c>
       <c r="M132">
         <f t="shared" si="11"/>
-        <v>9178</v>
+        <v>9191</v>
       </c>
       <c r="Y132">
-        <f t="shared" ref="Y132:Y195" si="16">ROUNDUP(SUM((-0.0949*B132)+18.0949),0)</f>
-        <v>6</v>
+        <f t="shared" ref="Y132:Y195" si="16">ROUNDUP(SUM((-0.09*B132)+18),0)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="2:25">
@@ -7459,7 +7464,7 @@
       </c>
       <c r="C133">
         <f t="shared" si="14"/>
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D133">
         <f t="shared" si="15"/>
@@ -7477,15 +7482,15 @@
       </c>
       <c r="K133">
         <f t="shared" si="13"/>
-        <v>5602</v>
+        <v>5610</v>
       </c>
       <c r="M133">
         <f t="shared" ref="M133:M196" si="17">ROUNDDOWN(SUM(1.1*((4*C133)+D133)*(H133/100)),0)</f>
-        <v>9337</v>
+        <v>9350</v>
       </c>
       <c r="Y133">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="2:25">
@@ -7494,7 +7499,7 @@
       </c>
       <c r="C134">
         <f t="shared" si="14"/>
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D134">
         <f t="shared" si="15"/>
@@ -7512,15 +7517,15 @@
       </c>
       <c r="K134">
         <f t="shared" si="13"/>
-        <v>5718</v>
+        <v>5726</v>
       </c>
       <c r="M134">
         <f t="shared" si="17"/>
-        <v>9531</v>
+        <v>9544</v>
       </c>
       <c r="Y134">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="2:25">
@@ -7529,7 +7534,7 @@
       </c>
       <c r="C135">
         <f t="shared" si="14"/>
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="D135">
         <f t="shared" si="15"/>
@@ -7547,15 +7552,15 @@
       </c>
       <c r="K135">
         <f t="shared" si="13"/>
-        <v>5815</v>
+        <v>5823</v>
       </c>
       <c r="M135">
         <f t="shared" si="17"/>
-        <v>9693</v>
+        <v>9706</v>
       </c>
       <c r="Y135">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="2:25">
@@ -7704,7 +7709,7 @@
       </c>
       <c r="C140">
         <f t="shared" si="14"/>
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D140">
         <f t="shared" si="15"/>
@@ -7722,15 +7727,15 @@
       </c>
       <c r="K140">
         <f t="shared" si="13"/>
-        <v>6329</v>
+        <v>6337</v>
       </c>
       <c r="M140">
         <f t="shared" si="17"/>
-        <v>10549</v>
+        <v>10563</v>
       </c>
       <c r="Y140">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="2:25">
@@ -7739,7 +7744,7 @@
       </c>
       <c r="C141">
         <f t="shared" si="14"/>
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D141">
         <f t="shared" si="15"/>
@@ -7757,15 +7762,15 @@
       </c>
       <c r="K141">
         <f t="shared" si="13"/>
-        <v>6450</v>
+        <v>6459</v>
       </c>
       <c r="M141">
         <f t="shared" si="17"/>
-        <v>10751</v>
+        <v>10766</v>
       </c>
       <c r="Y141">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" spans="2:25">
@@ -7774,7 +7779,7 @@
       </c>
       <c r="C142">
         <f t="shared" si="14"/>
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D142">
         <f t="shared" si="15"/>
@@ -7792,15 +7797,15 @@
       </c>
       <c r="K142">
         <f t="shared" si="13"/>
-        <v>6555</v>
+        <v>6564</v>
       </c>
       <c r="M142">
         <f t="shared" si="17"/>
-        <v>10926</v>
+        <v>10941</v>
       </c>
       <c r="Y142">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="2:25">
@@ -7809,7 +7814,7 @@
       </c>
       <c r="C143">
         <f t="shared" si="14"/>
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D143">
         <f t="shared" si="15"/>
@@ -7827,15 +7832,15 @@
       </c>
       <c r="K143">
         <f t="shared" si="13"/>
-        <v>6659</v>
+        <v>6667</v>
       </c>
       <c r="M143">
         <f t="shared" si="17"/>
-        <v>11099</v>
+        <v>11113</v>
       </c>
       <c r="Y143">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="2:25">
@@ -7844,7 +7849,7 @@
       </c>
       <c r="C144">
         <f t="shared" si="14"/>
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D144">
         <f t="shared" si="15"/>
@@ -7862,15 +7867,15 @@
       </c>
       <c r="K144">
         <f t="shared" si="13"/>
-        <v>6786</v>
+        <v>6795</v>
       </c>
       <c r="M144">
         <f t="shared" si="17"/>
-        <v>11310</v>
+        <v>11325</v>
       </c>
       <c r="Y144">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="2:25">
@@ -7879,7 +7884,7 @@
       </c>
       <c r="C145">
         <f t="shared" si="14"/>
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D145">
         <f t="shared" si="15"/>
@@ -7897,15 +7902,15 @@
       </c>
       <c r="K145">
         <f t="shared" si="13"/>
-        <v>6891</v>
+        <v>6900</v>
       </c>
       <c r="M145">
         <f t="shared" si="17"/>
-        <v>11485</v>
+        <v>11500</v>
       </c>
       <c r="Y145">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="2:25">
@@ -7914,7 +7919,7 @@
       </c>
       <c r="C146">
         <f t="shared" si="14"/>
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D146">
         <f t="shared" si="15"/>
@@ -7932,15 +7937,15 @@
       </c>
       <c r="K146">
         <f t="shared" si="13"/>
-        <v>7019</v>
+        <v>7029</v>
       </c>
       <c r="M146">
         <f t="shared" si="17"/>
-        <v>11699</v>
+        <v>11715</v>
       </c>
       <c r="Y146">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="2:25">
@@ -8089,7 +8094,7 @@
       </c>
       <c r="C151">
         <f t="shared" si="14"/>
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="D151">
         <f t="shared" si="15"/>
@@ -8107,15 +8112,15 @@
       </c>
       <c r="K151">
         <f t="shared" si="13"/>
-        <v>7599</v>
+        <v>7609</v>
       </c>
       <c r="M151">
         <f t="shared" si="17"/>
-        <v>12666</v>
+        <v>12682</v>
       </c>
       <c r="Y151">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="2:25">
@@ -8124,7 +8129,7 @@
       </c>
       <c r="C152">
         <f t="shared" si="14"/>
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D152">
         <f t="shared" si="15"/>
@@ -8142,15 +8147,15 @@
       </c>
       <c r="K152">
         <f t="shared" si="13"/>
-        <v>7734</v>
+        <v>7744</v>
       </c>
       <c r="M152">
         <f t="shared" si="17"/>
-        <v>12891</v>
+        <v>12907</v>
       </c>
       <c r="Y152">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="2:25">
@@ -8159,7 +8164,7 @@
       </c>
       <c r="C153">
         <f t="shared" si="14"/>
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D153">
         <f t="shared" si="15"/>
@@ -8177,15 +8182,15 @@
       </c>
       <c r="K153">
         <f t="shared" si="13"/>
-        <v>7846</v>
+        <v>7856</v>
       </c>
       <c r="M153">
         <f t="shared" si="17"/>
-        <v>13078</v>
+        <v>13094</v>
       </c>
       <c r="Y153">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="2:25">
@@ -8194,7 +8199,7 @@
       </c>
       <c r="C154">
         <f t="shared" si="14"/>
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D154">
         <f t="shared" si="15"/>
@@ -8212,15 +8217,15 @@
       </c>
       <c r="K154">
         <f t="shared" si="13"/>
-        <v>7983</v>
+        <v>7993</v>
       </c>
       <c r="M154">
         <f t="shared" si="17"/>
-        <v>13306</v>
+        <v>13322</v>
       </c>
       <c r="Y154">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="2:25">
@@ -8229,7 +8234,7 @@
       </c>
       <c r="C155">
         <f t="shared" si="14"/>
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D155">
         <f t="shared" si="15"/>
@@ -8247,15 +8252,15 @@
       </c>
       <c r="K155">
         <f t="shared" si="13"/>
-        <v>8097</v>
+        <v>8107</v>
       </c>
       <c r="M155">
         <f t="shared" si="17"/>
-        <v>13495</v>
+        <v>13512</v>
       </c>
       <c r="Y155">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="2:25">
@@ -8264,7 +8269,7 @@
       </c>
       <c r="C156">
         <f t="shared" si="14"/>
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D156">
         <f t="shared" si="15"/>
@@ -8282,15 +8287,15 @@
       </c>
       <c r="K156">
         <f t="shared" si="13"/>
-        <v>8236</v>
+        <v>8245</v>
       </c>
       <c r="M156">
         <f t="shared" si="17"/>
-        <v>13727</v>
+        <v>13743</v>
       </c>
       <c r="Y156">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="2:25">
@@ -8299,7 +8304,7 @@
       </c>
       <c r="C157">
         <f t="shared" si="14"/>
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="D157">
         <f t="shared" si="15"/>
@@ -8317,15 +8322,15 @@
       </c>
       <c r="K157">
         <f t="shared" si="13"/>
-        <v>8351</v>
+        <v>8361</v>
       </c>
       <c r="M157">
         <f t="shared" si="17"/>
-        <v>13919</v>
+        <v>13936</v>
       </c>
       <c r="Y157">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="2:25">
@@ -8474,7 +8479,7 @@
       </c>
       <c r="C162">
         <f t="shared" si="14"/>
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="D162">
         <f t="shared" si="15"/>
@@ -8492,15 +8497,15 @@
       </c>
       <c r="K162">
         <f t="shared" si="13"/>
-        <v>9028</v>
+        <v>9039</v>
       </c>
       <c r="M162">
         <f t="shared" si="17"/>
-        <v>15048</v>
+        <v>15065</v>
       </c>
       <c r="Y162">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="2:25">
@@ -8509,7 +8514,7 @@
       </c>
       <c r="C163">
         <f t="shared" si="14"/>
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D163">
         <f t="shared" si="15"/>
@@ -8527,15 +8532,15 @@
       </c>
       <c r="K163">
         <f t="shared" si="13"/>
-        <v>9149</v>
+        <v>9160</v>
       </c>
       <c r="M163">
         <f t="shared" si="17"/>
-        <v>15249</v>
+        <v>15267</v>
       </c>
       <c r="Y163">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="164" spans="2:25">
@@ -8544,7 +8549,7 @@
       </c>
       <c r="C164">
         <f t="shared" si="14"/>
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="D164">
         <f t="shared" si="15"/>
@@ -8562,15 +8567,15 @@
       </c>
       <c r="K164">
         <f t="shared" si="13"/>
-        <v>9296</v>
+        <v>9307</v>
       </c>
       <c r="M164">
         <f t="shared" si="17"/>
-        <v>15494</v>
+        <v>15512</v>
       </c>
       <c r="Y164">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165" spans="2:25">
@@ -8579,7 +8584,7 @@
       </c>
       <c r="C165">
         <f t="shared" si="14"/>
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D165">
         <f t="shared" si="15"/>
@@ -8597,15 +8602,15 @@
       </c>
       <c r="K165">
         <f t="shared" si="13"/>
-        <v>9441</v>
+        <v>9453</v>
       </c>
       <c r="M165">
         <f t="shared" si="17"/>
-        <v>15736</v>
+        <v>15755</v>
       </c>
       <c r="Y165">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="2:25">
@@ -8614,7 +8619,7 @@
       </c>
       <c r="C166">
         <f t="shared" si="14"/>
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="D166">
         <f t="shared" si="15"/>
@@ -8632,15 +8637,15 @@
       </c>
       <c r="K166">
         <f t="shared" ref="K166:K202" si="21">ROUNDDOWN(SUM(0.6*M166),0)</f>
-        <v>9591</v>
+        <v>9602</v>
       </c>
       <c r="M166">
         <f t="shared" si="17"/>
-        <v>15985</v>
+        <v>16004</v>
       </c>
       <c r="Y166">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="2:25">
@@ -8649,7 +8654,7 @@
       </c>
       <c r="C167">
         <f t="shared" si="14"/>
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D167">
         <f t="shared" si="15"/>
@@ -8667,15 +8672,15 @@
       </c>
       <c r="K167">
         <f t="shared" si="21"/>
-        <v>9715</v>
+        <v>9726</v>
       </c>
       <c r="M167">
         <f t="shared" si="17"/>
-        <v>16193</v>
+        <v>16211</v>
       </c>
       <c r="Y167">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="2:25">
@@ -8684,7 +8689,7 @@
       </c>
       <c r="C168">
         <f t="shared" si="14"/>
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D168">
         <f t="shared" si="15"/>
@@ -8702,15 +8707,15 @@
       </c>
       <c r="K168">
         <f t="shared" si="21"/>
-        <v>9867</v>
+        <v>9877</v>
       </c>
       <c r="M168">
         <f t="shared" si="17"/>
-        <v>16445</v>
+        <v>16463</v>
       </c>
       <c r="Y168">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="2:25">
@@ -8824,7 +8829,7 @@
       </c>
       <c r="C172">
         <f t="shared" si="14"/>
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D172">
         <f t="shared" si="15"/>
@@ -8842,15 +8847,15 @@
       </c>
       <c r="K172">
         <f t="shared" si="21"/>
-        <v>10441</v>
+        <v>10453</v>
       </c>
       <c r="M172">
         <f t="shared" si="17"/>
-        <v>17403</v>
+        <v>17423</v>
       </c>
       <c r="Y172">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="2:25">
@@ -8859,7 +8864,7 @@
       </c>
       <c r="C173">
         <f t="shared" si="14"/>
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="D173">
         <f t="shared" si="15"/>
@@ -8877,15 +8882,15 @@
       </c>
       <c r="K173">
         <f t="shared" si="21"/>
-        <v>10595</v>
+        <v>10607</v>
       </c>
       <c r="M173">
         <f t="shared" si="17"/>
-        <v>17659</v>
+        <v>17679</v>
       </c>
       <c r="Y173">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="2:25">
@@ -8894,7 +8899,7 @@
       </c>
       <c r="C174">
         <f t="shared" si="14"/>
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D174">
         <f t="shared" si="15"/>
@@ -8912,15 +8917,15 @@
       </c>
       <c r="K174">
         <f t="shared" si="21"/>
-        <v>10753</v>
+        <v>10765</v>
       </c>
       <c r="M174">
         <f t="shared" si="17"/>
-        <v>17922</v>
+        <v>17942</v>
       </c>
       <c r="Y174">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="2:25">
@@ -8929,7 +8934,7 @@
       </c>
       <c r="C175">
         <f t="shared" si="14"/>
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="D175">
         <f t="shared" si="15"/>
@@ -8947,15 +8952,15 @@
       </c>
       <c r="K175">
         <f t="shared" si="21"/>
-        <v>10909</v>
+        <v>10920</v>
       </c>
       <c r="M175">
         <f t="shared" si="17"/>
-        <v>18182</v>
+        <v>18201</v>
       </c>
       <c r="Y175">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="2:25">
@@ -8964,7 +8969,7 @@
       </c>
       <c r="C176">
         <f t="shared" si="14"/>
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="D176">
         <f t="shared" si="15"/>
@@ -8982,15 +8987,15 @@
       </c>
       <c r="K176">
         <f t="shared" si="21"/>
-        <v>11068</v>
+        <v>11080</v>
       </c>
       <c r="M176">
         <f t="shared" si="17"/>
-        <v>18448</v>
+        <v>18468</v>
       </c>
       <c r="Y176">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" spans="2:25">
@@ -8999,7 +9004,7 @@
       </c>
       <c r="C177">
         <f t="shared" si="14"/>
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D177">
         <f t="shared" si="15"/>
@@ -9017,15 +9022,15 @@
       </c>
       <c r="K177">
         <f t="shared" si="21"/>
-        <v>11226</v>
+        <v>11238</v>
       </c>
       <c r="M177">
         <f t="shared" si="17"/>
-        <v>18711</v>
+        <v>18731</v>
       </c>
       <c r="Y177">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="2:25">
@@ -9034,7 +9039,7 @@
       </c>
       <c r="C178">
         <f t="shared" si="14"/>
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="D178">
         <f t="shared" si="15"/>
@@ -9052,15 +9057,15 @@
       </c>
       <c r="K178">
         <f t="shared" si="21"/>
-        <v>11388</v>
+        <v>11400</v>
       </c>
       <c r="M178">
         <f t="shared" si="17"/>
-        <v>18981</v>
+        <v>19001</v>
       </c>
       <c r="Y178">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="2:25">
@@ -9069,7 +9074,7 @@
       </c>
       <c r="C179">
         <f t="shared" si="14"/>
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D179">
         <f t="shared" si="15"/>
@@ -9087,15 +9092,15 @@
       </c>
       <c r="K179">
         <f t="shared" si="21"/>
-        <v>11548</v>
+        <v>11560</v>
       </c>
       <c r="M179">
         <f t="shared" si="17"/>
-        <v>19248</v>
+        <v>19268</v>
       </c>
       <c r="Y179">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="2:25">
@@ -9209,7 +9214,7 @@
       </c>
       <c r="C183">
         <f t="shared" si="22"/>
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="D183">
         <f t="shared" si="23"/>
@@ -9227,15 +9232,15 @@
       </c>
       <c r="K183">
         <f t="shared" si="21"/>
-        <v>12193</v>
+        <v>12205</v>
       </c>
       <c r="M183">
         <f t="shared" si="17"/>
-        <v>20322</v>
+        <v>20343</v>
       </c>
       <c r="Y183">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="2:25">
@@ -9244,7 +9249,7 @@
       </c>
       <c r="C184">
         <f t="shared" si="22"/>
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="D184">
         <f t="shared" si="23"/>
@@ -9262,15 +9267,15 @@
       </c>
       <c r="K184">
         <f t="shared" si="21"/>
-        <v>12361</v>
+        <v>12374</v>
       </c>
       <c r="M184">
         <f t="shared" si="17"/>
-        <v>20603</v>
+        <v>20624</v>
       </c>
       <c r="Y184">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="2:25">
@@ -9279,7 +9284,7 @@
       </c>
       <c r="C185">
         <f t="shared" si="22"/>
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D185">
         <f t="shared" si="23"/>
@@ -9297,15 +9302,15 @@
       </c>
       <c r="K185">
         <f t="shared" si="21"/>
-        <v>12528</v>
+        <v>12540</v>
       </c>
       <c r="M185">
         <f t="shared" si="17"/>
-        <v>20880</v>
+        <v>20901</v>
       </c>
       <c r="Y185">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="2:25">
@@ -9314,7 +9319,7 @@
       </c>
       <c r="C186">
         <f t="shared" si="22"/>
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D186">
         <f t="shared" si="23"/>
@@ -9332,15 +9337,15 @@
       </c>
       <c r="K186">
         <f t="shared" si="21"/>
-        <v>12698</v>
+        <v>12711</v>
       </c>
       <c r="M186">
         <f t="shared" si="17"/>
-        <v>21164</v>
+        <v>21186</v>
       </c>
       <c r="Y186">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="2:25">
@@ -9349,7 +9354,7 @@
       </c>
       <c r="C187">
         <f t="shared" si="22"/>
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="D187">
         <f t="shared" si="23"/>
@@ -9367,15 +9372,15 @@
       </c>
       <c r="K187">
         <f t="shared" si="21"/>
-        <v>12867</v>
+        <v>12880</v>
       </c>
       <c r="M187">
         <f t="shared" si="17"/>
-        <v>21445</v>
+        <v>21467</v>
       </c>
       <c r="Y187">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="2:25">
@@ -9384,7 +9389,7 @@
       </c>
       <c r="C188">
         <f t="shared" si="22"/>
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="D188">
         <f t="shared" si="23"/>
@@ -9402,15 +9407,15 @@
       </c>
       <c r="K188">
         <f t="shared" si="21"/>
-        <v>13039</v>
+        <v>13053</v>
       </c>
       <c r="M188">
         <f t="shared" si="17"/>
-        <v>21733</v>
+        <v>21755</v>
       </c>
       <c r="Y188">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="2:25">
@@ -9419,7 +9424,7 @@
       </c>
       <c r="C189">
         <f t="shared" si="22"/>
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D189">
         <f t="shared" si="23"/>
@@ -9437,15 +9442,15 @@
       </c>
       <c r="K189">
         <f t="shared" si="21"/>
-        <v>13210</v>
+        <v>13224</v>
       </c>
       <c r="M189">
         <f t="shared" si="17"/>
-        <v>22017</v>
+        <v>22040</v>
       </c>
       <c r="Y189">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="2:25">
@@ -9454,7 +9459,7 @@
       </c>
       <c r="C190">
         <f t="shared" si="22"/>
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D190">
         <f t="shared" si="23"/>
@@ -9472,15 +9477,15 @@
       </c>
       <c r="K190">
         <f t="shared" si="21"/>
-        <v>13385</v>
+        <v>13399</v>
       </c>
       <c r="M190">
         <f t="shared" si="17"/>
-        <v>22309</v>
+        <v>22332</v>
       </c>
       <c r="Y190">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="2:25">
@@ -9559,7 +9564,7 @@
       </c>
       <c r="C193">
         <f t="shared" si="22"/>
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="D193">
         <f t="shared" si="23"/>
@@ -9577,15 +9582,15 @@
       </c>
       <c r="K193">
         <f t="shared" si="21"/>
-        <v>13909</v>
+        <v>13936</v>
       </c>
       <c r="M193">
         <f t="shared" si="17"/>
-        <v>23182</v>
+        <v>23228</v>
       </c>
       <c r="Y193">
         <f t="shared" si="16"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="2:25">
@@ -9594,7 +9599,7 @@
       </c>
       <c r="C194">
         <f t="shared" si="22"/>
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="D194">
         <f t="shared" si="23"/>
@@ -9612,15 +9617,15 @@
       </c>
       <c r="K194">
         <f t="shared" si="21"/>
-        <v>14088</v>
+        <v>14116</v>
       </c>
       <c r="M194">
         <f t="shared" si="17"/>
-        <v>23481</v>
+        <v>23528</v>
       </c>
       <c r="Y194">
         <f t="shared" si="16"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="2:25">
@@ -9629,7 +9634,7 @@
       </c>
       <c r="C195">
         <f t="shared" si="22"/>
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="D195">
         <f t="shared" si="23"/>
@@ -9647,15 +9652,15 @@
       </c>
       <c r="K195">
         <f t="shared" si="21"/>
-        <v>14265</v>
+        <v>14293</v>
       </c>
       <c r="M195">
         <f t="shared" si="17"/>
-        <v>23776</v>
+        <v>23823</v>
       </c>
       <c r="Y195">
         <f t="shared" si="16"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="2:25">
@@ -9664,7 +9669,7 @@
       </c>
       <c r="C196">
         <f t="shared" si="22"/>
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D196">
         <f t="shared" si="23"/>
@@ -9682,15 +9687,15 @@
       </c>
       <c r="K196">
         <f t="shared" si="21"/>
-        <v>14447</v>
+        <v>14475</v>
       </c>
       <c r="M196">
         <f t="shared" si="17"/>
-        <v>24079</v>
+        <v>24126</v>
       </c>
       <c r="Y196">
-        <f t="shared" ref="Y196:Y202" si="24">ROUNDUP(SUM((-0.0949*B196)+18.0949),0)</f>
-        <v>-1</v>
+        <f t="shared" ref="Y196:Y202" si="24">ROUNDUP(SUM((-0.09*B196)+18),0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="2:25">
@@ -9699,7 +9704,7 @@
       </c>
       <c r="C197">
         <f t="shared" si="22"/>
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="D197">
         <f t="shared" si="23"/>
@@ -9717,15 +9722,15 @@
       </c>
       <c r="K197">
         <f t="shared" si="21"/>
-        <v>14653</v>
+        <v>14682</v>
       </c>
       <c r="M197">
         <f t="shared" ref="M197:M202" si="25">ROUNDDOWN(SUM(1.1*((4*C197)+D197)*(H197/100)),0)</f>
-        <v>24422</v>
+        <v>24470</v>
       </c>
       <c r="Y197">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="2:25">
@@ -9733,12 +9738,10 @@
         <v>196</v>
       </c>
       <c r="C198">
-        <f t="shared" si="22"/>
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="D198">
-        <f t="shared" si="23"/>
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E198">
         <v>4</v>
@@ -9752,15 +9755,15 @@
       </c>
       <c r="K198">
         <f t="shared" si="21"/>
-        <v>14837</v>
+        <v>14812</v>
       </c>
       <c r="M198">
         <f t="shared" si="25"/>
-        <v>24729</v>
+        <v>24687</v>
       </c>
       <c r="Y198">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="2:25">
@@ -9768,12 +9771,10 @@
         <v>197</v>
       </c>
       <c r="C199">
-        <f t="shared" si="22"/>
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="D199">
-        <f t="shared" si="23"/>
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E199">
         <v>4</v>
@@ -9787,15 +9788,15 @@
       </c>
       <c r="K199">
         <f t="shared" si="21"/>
-        <v>15018</v>
+        <v>14938</v>
       </c>
       <c r="M199">
         <f t="shared" si="25"/>
-        <v>25031</v>
+        <v>24898</v>
       </c>
       <c r="Y199">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="2:25">
@@ -9803,12 +9804,10 @@
         <v>198</v>
       </c>
       <c r="C200">
-        <f t="shared" si="22"/>
-        <v>1012</v>
+        <v>999</v>
       </c>
       <c r="D200">
-        <f t="shared" si="23"/>
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="E200">
         <v>4</v>
@@ -9822,15 +9821,15 @@
       </c>
       <c r="K200">
         <f t="shared" si="21"/>
-        <v>15204</v>
+        <v>15069</v>
       </c>
       <c r="M200">
         <f t="shared" si="25"/>
-        <v>25341</v>
+        <v>25116</v>
       </c>
       <c r="Y200">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="2:25">
@@ -9838,12 +9837,10 @@
         <v>199</v>
       </c>
       <c r="C201">
-        <f t="shared" si="22"/>
-        <v>1017</v>
+        <v>999</v>
       </c>
       <c r="D201">
-        <f t="shared" si="23"/>
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="E201">
         <v>4</v>
@@ -9857,15 +9854,15 @@
       </c>
       <c r="K201">
         <f t="shared" si="21"/>
-        <v>15415</v>
+        <v>15228</v>
       </c>
       <c r="M201">
         <f t="shared" si="25"/>
-        <v>25693</v>
+        <v>25380</v>
       </c>
       <c r="Y201">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="2:25">
@@ -9873,12 +9870,10 @@
         <v>200</v>
       </c>
       <c r="C202">
-        <f t="shared" si="22"/>
-        <v>1022</v>
+        <v>999</v>
       </c>
       <c r="D202">
-        <f t="shared" si="23"/>
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="E202">
         <v>4</v>
@@ -9892,15 +9887,15 @@
       </c>
       <c r="K202">
         <f t="shared" si="21"/>
-        <v>15604</v>
+        <v>15355</v>
       </c>
       <c r="M202">
         <f t="shared" si="25"/>
-        <v>26007</v>
+        <v>25593</v>
       </c>
       <c r="Y202">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>